<commit_message>
ajout des taux de change
</commit_message>
<xml_diff>
--- a/DataFeeds/StocksName.xlsx
+++ b/DataFeeds/StocksName.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="StockData" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
   <si>
     <t>CompleteName</t>
   </si>
@@ -344,8 +344,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-m\-d;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-m\-d;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -356,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -405,6 +405,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -418,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -428,8 +434,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,15 +738,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -759,7 +766,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -776,7 +783,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -793,7 +800,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -810,7 +817,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -827,7 +834,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -844,7 +851,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -867,51 +874,59 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="2"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>49</v>
+      </c>
       <c r="H8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="H9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>53</v>
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
         <v>49</v>
@@ -920,29 +935,27 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>55</v>
-      </c>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="H11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>49</v>
@@ -952,35 +965,27 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="H13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>49</v>
@@ -990,27 +995,45 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="4"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1"/>
       <c r="H15" t="s">
+        <v>75</v>
+      </c>
+      <c r="L15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>77</v>
+      </c>
+      <c r="N15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15" t="s">
+        <v>84</v>
+      </c>
+      <c r="P15" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>49</v>
@@ -1019,13 +1042,31 @@
       <c r="H16" t="s">
         <v>75</v>
       </c>
+      <c r="L16">
+        <v>17</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>7</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>49</v>
@@ -1037,10 +1078,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>49</v>
@@ -1051,75 +1092,77 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="2"/>
+      <c r="A19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H19" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20" s="1"/>
+      <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="H20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>52</v>
-      </c>
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="5"/>
       <c r="H21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>52</v>
+      <c r="A22" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="H22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>79</v>
@@ -1130,33 +1173,33 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="1"/>
+      <c r="A24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="2"/>
       <c r="H24" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="6"/>
+      <c r="A25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="2"/>
       <c r="H25" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1183,66 +1226,84 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="1"/>
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="H27" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D28" s="2"/>
+      <c r="H28" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="1"/>
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="H29" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="2"/>
+      <c r="A30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="H30" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D31" s="2"/>
+      <c r="A31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="H31" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A1:H31">
+    <sortCondition descending="1" ref="H1:H31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -1253,7 +1314,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,13 +1375,13 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1336,13 +1397,13 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1388,7 +1449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>